<commit_message>
EPBDS-10194 Cast from Spreadsheat to Spreadsheet[] is not happening if spreadsheets are different
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9461_Spreadshet_Array_conversion_typeLoss_check.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9461_Spreadshet_Array_conversion_typeLoss_check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="22430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\demo2\openl-demo\user-workspace\DEFAULT\Spr_convert_bug\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B95BEF07-1272-4C2E-9CC1-09DBF7A9AE21}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB07D9A3-E41C-4ABE-91DB-E0A97E978C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2475" yWindow="915" windowWidth="24420" windowHeight="13575" xr2:uid="{47A14633-2726-4551-8D95-1D1906557466}"/>
+    <workbookView xWindow="8160" yWindow="2170" windowWidth="22680" windowHeight="17060" xr2:uid="{47A14633-2726-4551-8D95-1D1906557466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,14 +20,6 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:Single"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:CNMTM"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
@@ -239,7 +231,7 @@
     <t>1, 1.2</t>
   </si>
   <si>
-    <t>Object[]</t>
+    <t>Serializable[]</t>
   </si>
 </sst>
 </file>
@@ -366,7 +358,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -382,9 +374,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Тема Office">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Стандартная">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -422,7 +414,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Стандартная">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -528,7 +520,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Стандартная">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -680,28 +672,28 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DE773D-551D-4638-97B8-E9452808D335}">
   <dimension ref="B2:P75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A56" workbookViewId="0">
-      <selection activeCell="J73" sqref="J73"/>
+    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
+      <selection activeCell="L79" sqref="L79"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="32.42578125" customWidth="1" collapsed="1"/>
-    <col min="3" max="3" width="39.7109375" customWidth="1" collapsed="1"/>
-    <col min="4" max="4" width="14.5703125" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="31.5703125" customWidth="1" collapsed="1"/>
-    <col min="8" max="8" width="33.7109375" customWidth="1" collapsed="1"/>
+    <col min="2" max="2" width="32.453125" customWidth="1" collapsed="1"/>
+    <col min="3" max="3" width="39.7265625" customWidth="1" collapsed="1"/>
+    <col min="4" max="4" width="14.54296875" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="31.54296875" customWidth="1" collapsed="1"/>
+    <col min="8" max="8" width="33.7265625" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="24" customWidth="1" collapsed="1"/>
-    <col min="14" max="14" width="21.140625" customWidth="1" collapsed="1"/>
-    <col min="15" max="15" width="20.42578125" customWidth="1" collapsed="1"/>
+    <col min="14" max="14" width="21.1796875" customWidth="1" collapsed="1"/>
+    <col min="15" max="15" width="20.453125" customWidth="1" collapsed="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:8" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="2" spans="2:8" ht="26" x14ac:dyDescent="0.6">
       <c r="B2" s="3" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B5" s="4" t="s">
         <v>3</v>
       </c>
@@ -709,7 +701,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B6" s="4" t="s">
         <v>0</v>
       </c>
@@ -717,7 +709,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B7" s="4" t="s">
         <v>1</v>
       </c>
@@ -725,7 +717,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B8" s="4" t="s">
         <v>2</v>
       </c>
@@ -733,7 +725,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B12" s="7" t="s">
         <v>8</v>
       </c>
@@ -743,7 +735,7 @@
       </c>
       <c r="H12" s="7"/>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B13" s="4" t="s">
         <v>9</v>
       </c>
@@ -757,7 +749,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B14" s="4" t="s">
         <v>11</v>
       </c>
@@ -771,7 +763,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B15" s="4" t="s">
         <v>12</v>
       </c>
@@ -785,7 +777,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.35">
       <c r="B16" s="4" t="s">
         <v>13</v>
       </c>
@@ -799,7 +791,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B17" s="4" t="s">
         <v>24</v>
       </c>
@@ -813,11 +805,11 @@
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B19" s="9" t="s">
         <v>53</v>
       </c>
@@ -830,7 +822,7 @@
       <c r="I19" s="7"/>
       <c r="J19" s="7"/>
     </row>
-    <row r="20" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B20" s="4" t="s">
         <v>49</v>
       </c>
@@ -853,7 +845,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B21" s="4" t="s">
         <v>49</v>
       </c>
@@ -876,7 +868,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="B22" s="4">
         <v>1</v>
       </c>
@@ -899,21 +891,21 @@
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="27" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G27" s="7" t="s">
         <v>35</v>
       </c>
       <c r="H27" s="7"/>
     </row>
-    <row r="28" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G28" s="4" t="s">
         <v>9</v>
       </c>
@@ -921,7 +913,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D29"/>
       <c r="G29" s="4" t="s">
         <v>11</v>
@@ -931,7 +923,7 @@
       </c>
       <c r="I29"/>
     </row>
-    <row r="30" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:10" x14ac:dyDescent="0.35">
       <c r="G30" s="4" t="s">
         <v>12</v>
       </c>
@@ -940,7 +932,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="G31" s="4" t="s">
         <v>13</v>
       </c>
@@ -949,7 +941,7 @@
       </c>
       <c r="I31"/>
     </row>
-    <row r="32" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="D32"/>
       <c r="G32" s="4" t="s">
         <v>24</v>
@@ -958,20 +950,20 @@
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="G35" s="8" t="s">
         <v>56</v>
       </c>
       <c r="H35" s="8"/>
       <c r="I35" s="8"/>
     </row>
-    <row r="36" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="G36" s="6" t="s">
         <v>49</v>
       </c>
@@ -988,7 +980,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="G37" s="6" t="s">
         <v>49</v>
       </c>
@@ -1005,7 +997,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="38" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
       <c r="G38" s="4" t="s">
         <v>42</v>
       </c>
@@ -1022,13 +1014,13 @@
         <v>62</v>
       </c>
     </row>
-    <row r="39" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.25"/>
-    <row r="42" spans="2:11" ht="26.25" x14ac:dyDescent="0.4">
+    <row r="39" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
+    <row r="42" spans="2:11" ht="26" x14ac:dyDescent="0.6">
       <c r="B42" s="3" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B45" s="7" t="s">
         <v>17</v>
       </c>
@@ -1038,7 +1030,7 @@
       </c>
       <c r="H45" s="7"/>
     </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B46" s="4" t="s">
         <v>18</v>
       </c>
@@ -1052,7 +1044,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B47" s="4" t="s">
         <v>20</v>
       </c>
@@ -1066,7 +1058,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="52" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B52" s="7" t="s">
         <v>27</v>
       </c>
@@ -1079,7 +1071,7 @@
       </c>
       <c r="H52" s="7"/>
     </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="53" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B53" s="4" t="s">
         <v>18</v>
       </c>
@@ -1096,7 +1088,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="54" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B54" s="4" t="s">
         <v>29</v>
       </c>
@@ -1113,14 +1105,14 @@
         <v>38</v>
       </c>
     </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="56" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B56" s="7" t="s">
         <v>31</v>
       </c>
       <c r="C56" s="7"/>
       <c r="P56" s="2"/>
     </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="57" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B57" s="4" t="s">
         <v>9</v>
       </c>
@@ -1134,7 +1126,7 @@
       <c r="I57" s="7"/>
       <c r="J57" s="7"/>
     </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="58" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B58" s="4" t="s">
         <v>11</v>
       </c>
@@ -1157,7 +1149,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="59" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B59" s="4" t="s">
         <v>12</v>
       </c>
@@ -1180,7 +1172,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="60" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B60" s="4" t="s">
         <v>13</v>
       </c>
@@ -1203,7 +1195,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="61" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B61" s="4" t="s">
         <v>24</v>
       </c>
@@ -1211,7 +1203,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="63" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B63" s="7" t="s">
         <v>26</v>
       </c>
@@ -1225,7 +1217,7 @@
       <c r="I63" s="7"/>
       <c r="J63" s="7"/>
     </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.25">
+    <row r="64" spans="2:16" x14ac:dyDescent="0.35">
       <c r="B64" s="4" t="s">
         <v>9</v>
       </c>
@@ -1245,7 +1237,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B65" s="4" t="s">
         <v>11</v>
       </c>
@@ -1265,7 +1257,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B66" s="4" t="s">
         <v>12</v>
       </c>
@@ -1285,7 +1277,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B67" s="4" t="s">
         <v>13</v>
       </c>
@@ -1293,7 +1285,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="68" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B68" s="4" t="s">
         <v>24</v>
       </c>
@@ -1301,7 +1293,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B70" s="7" t="s">
         <v>59</v>
       </c>
@@ -1313,7 +1305,7 @@
       <c r="I70" s="7"/>
       <c r="J70" s="7"/>
     </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B71" s="4" t="s">
         <v>9</v>
       </c>
@@ -1333,7 +1325,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B72" s="4" t="s">
         <v>11</v>
       </c>
@@ -1353,7 +1345,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B73" s="4" t="s">
         <v>12</v>
       </c>
@@ -1373,7 +1365,7 @@
         <v>68</v>
       </c>
     </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B74" s="4" t="s">
         <v>13</v>
       </c>
@@ -1381,7 +1373,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B75" s="4" t="s">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
EPBDS-10708 Fix Java 15 build
--HG--
branch : 5.23.x
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9461_Spreadshet_Array_conversion_typeLoss_check.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9461_Spreadshet_Array_conversion_typeLoss_check.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB07D9A3-E41C-4ABE-91DB-E0A97E978C58}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C206D5D-65C0-40BF-B8FD-5DFD0D15BF94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="8160" yWindow="2170" windowWidth="22680" windowHeight="17060" xr2:uid="{47A14633-2726-4551-8D95-1D1906557466}"/>
   </bookViews>
@@ -231,7 +231,7 @@
     <t>1, 1.2</t>
   </si>
   <si>
-    <t>Serializable[]</t>
+    <t>Object[]</t>
   </si>
 </sst>
 </file>
@@ -673,7 +673,7 @@
   <dimension ref="B2:P75"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="L79" sqref="L79"/>
+      <selection activeCell="G51" sqref="G51"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
EPBDS-13112 No error is presented if unexisting method is called, and Alias exists in the project with the name = method name
</commit_message>
<xml_diff>
--- a/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9461_Spreadshet_Array_conversion_typeLoss_check.xlsx
+++ b/STUDIO/org.openl.rules.test/test-resources/functionality/EPBDS-9461_Spreadshet_Array_conversion_typeLoss_check.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="23328"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="25831"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\OPENL\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Projects\openl-tablets\STUDIO\org.openl.rules.test\test-resources\functionality\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C206D5D-65C0-40BF-B8FD-5DFD0D15BF94}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D849EA5C-2C8B-4D54-9E5B-8BAFB5289EC6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8160" yWindow="2170" windowWidth="22680" windowHeight="17060" xr2:uid="{47A14633-2726-4551-8D95-1D1906557466}"/>
+    <workbookView xWindow="4630" yWindow="3350" windowWidth="21550" windowHeight="15720" xr2:uid="{47A14633-2726-4551-8D95-1D1906557466}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -189,12 +189,6 @@
     <t>Test datatypeConvert</t>
   </si>
   <si>
-    <t>=new MyAlias1("aaa")</t>
-  </si>
-  <si>
-    <t>=new MyAlias2("eee")</t>
-  </si>
-  <si>
     <t>Test datatypeConvert3Arr</t>
   </si>
   <si>
@@ -232,6 +226,12 @@
   </si>
   <si>
     <t>Object[]</t>
+  </si>
+  <si>
+    <t>= (MyAlias1) "aaa"</t>
+  </si>
+  <si>
+    <t>= (MyAlias2) "eee"</t>
   </si>
 </sst>
 </file>
@@ -333,18 +333,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="12">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
@@ -670,10 +665,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0DE773D-551D-4638-97B8-E9452808D335}">
-  <dimension ref="B2:P75"/>
+  <dimension ref="B2:O75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D43" workbookViewId="0">
-      <selection activeCell="G51" sqref="G51"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -689,695 +684,679 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" ht="26" x14ac:dyDescent="0.6">
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>15</v>
       </c>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B5" s="4" t="s">
+      <c r="B5" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="G5" s="4" t="s">
+      <c r="G5" s="3" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B6" s="4" t="s">
+      <c r="B6" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="G6" s="4" t="s">
+      <c r="G6" s="3" t="s">
         <v>4</v>
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B7" s="4" t="s">
+      <c r="B7" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="G7" s="4" t="s">
+      <c r="G7" s="3" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B8" s="4" t="s">
+      <c r="B8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="G8" s="4" t="s">
+      <c r="G8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B12" s="7" t="s">
+      <c r="B12" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="C12" s="7"/>
-      <c r="G12" s="7" t="s">
+      <c r="C12" s="5"/>
+      <c r="G12" s="5" t="s">
         <v>32</v>
       </c>
-      <c r="H12" s="7"/>
+      <c r="H12" s="5"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B13" s="4" t="s">
+      <c r="B13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="C13" s="4" t="s">
+      <c r="C13" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="G13" s="4" t="s">
+      <c r="G13" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H13" s="4" t="s">
+      <c r="H13" s="3" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B14" s="4" t="s">
+      <c r="B14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C14" s="5" t="s">
-        <v>54</v>
-      </c>
-      <c r="G14" s="4" t="s">
+      <c r="C14" s="4" t="s">
+        <v>67</v>
+      </c>
+      <c r="G14" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H14" s="5" t="s">
+      <c r="H14" s="4" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B15" s="4" t="s">
+      <c r="B15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C15" s="5" t="s">
-        <v>55</v>
-      </c>
-      <c r="G15" s="4" t="s">
+      <c r="C15" s="4" t="s">
+        <v>68</v>
+      </c>
+      <c r="G15" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H15" s="5" t="s">
+      <c r="H15" s="4" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.35">
-      <c r="B16" s="4" t="s">
+      <c r="B16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C16" s="5" t="s">
+      <c r="C16" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H16" s="5" t="s">
+      <c r="H16" s="4" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="17" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="4" t="s">
+    <row r="17" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C17" s="5" t="s">
+      <c r="C17" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="G17" s="4" t="s">
+      <c r="G17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H17" s="5" t="s">
+      <c r="H17" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="18" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B19" s="9" t="s">
+    <row r="19" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B19" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="G19" s="7" t="s">
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="G19" s="5" t="s">
         <v>48</v>
       </c>
-      <c r="H19" s="7"/>
-      <c r="I19" s="7"/>
-      <c r="J19" s="7"/>
-    </row>
-    <row r="20" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B20" s="4" t="s">
+      <c r="H19" s="5"/>
+      <c r="I19" s="5"/>
+      <c r="J19" s="5"/>
+    </row>
+    <row r="20" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C20" s="4" t="s">
+      <c r="C20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D20" s="4" t="s">
+      <c r="D20" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H20" s="4" t="s">
+      <c r="H20" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I20" s="4" t="s">
+      <c r="I20" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J20" s="4" t="s">
+      <c r="J20" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="21" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B21" s="4" t="s">
+    <row r="21" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="C21" s="4" t="s">
+      <c r="C21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="D21" s="4" t="s">
+      <c r="D21" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="G21" s="4" t="s">
+      <c r="G21" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="I21" s="4" t="s">
+      <c r="I21" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="J21" s="4" t="s">
+      <c r="J21" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="22" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="B22" s="4">
+    <row r="22" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B22" s="3">
         <v>1</v>
       </c>
-      <c r="C22" s="4" t="s">
+      <c r="C22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="D22" s="4" t="s">
+      <c r="D22" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="G22" s="4" t="s">
+      <c r="G22" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="I22" s="4" t="s">
+      <c r="I22" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="J22" s="4" t="s">
+      <c r="J22" s="3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="23" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="C24" s="1"/>
       <c r="H24" s="1"/>
     </row>
     <row r="27" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G27" s="7" t="s">
+      <c r="G27" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="H27" s="7"/>
+      <c r="H27" s="5"/>
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G28" s="4" t="s">
+      <c r="G28" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="H28" s="4" t="s">
+      <c r="H28" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="29" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D29"/>
-      <c r="G29" s="4" t="s">
+    <row r="29" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="G29" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="H29" s="5" t="s">
+      <c r="H29" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="I29"/>
     </row>
     <row r="30" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="G30" s="4" t="s">
+      <c r="G30" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="H30" s="5" t="s">
+      <c r="H30" s="4" t="s">
         <v>34</v>
       </c>
-      <c r="I30" s="2"/>
-    </row>
-    <row r="31" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="G31" s="4" t="s">
+    </row>
+    <row r="31" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="G31" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="H31" s="5" t="s">
+      <c r="H31" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="I31"/>
-    </row>
-    <row r="32" spans="2:10" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="D32"/>
-      <c r="G32" s="4" t="s">
+    </row>
+    <row r="32" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="G32" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="H32" s="5" t="s">
+      <c r="H32" s="4" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="33" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C33" s="1"/>
     </row>
-    <row r="34" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="34" spans="2:11" x14ac:dyDescent="0.35">
       <c r="C34" s="1"/>
     </row>
-    <row r="35" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="G35" s="8" t="s">
+    <row r="35" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="G35" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="H35" s="5"/>
+      <c r="I35" s="5"/>
+    </row>
+    <row r="36" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="G36" t="s">
+        <v>49</v>
+      </c>
+      <c r="H36" t="s">
+        <v>50</v>
+      </c>
+      <c r="I36" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J36" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K36" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="37" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="G37" t="s">
+        <v>49</v>
+      </c>
+      <c r="H37" t="s">
+        <v>50</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K37" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="G38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I38" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J38" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K38" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="26" x14ac:dyDescent="0.6">
+      <c r="B42" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B45" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="C45" s="5"/>
+      <c r="G45" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="H45" s="5"/>
+    </row>
+    <row r="46" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C46" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G46" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H46" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="47" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B47" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C47" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G47" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="H47" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B52" s="5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C52" s="5"/>
+      <c r="G52" s="5" t="s">
+        <v>28</v>
+      </c>
+      <c r="H52" s="5"/>
+    </row>
+    <row r="53" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C53" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G53" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="H53" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="54" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B54" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="C54" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="G54" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H54" s="3" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B56" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C56" s="5"/>
+    </row>
+    <row r="57" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B57" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C57" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H57" s="5"/>
+      <c r="I57" s="5"/>
+      <c r="J57" s="5"/>
+    </row>
+    <row r="58" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B58" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G58" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H58" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I58" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J58" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K58" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="59" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B59" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C59" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G59" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H59" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I59" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="J59" s="3" t="s">
+        <v>59</v>
+      </c>
+      <c r="K59" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="60" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B60" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C60" s="4" t="s">
+        <v>14</v>
+      </c>
+      <c r="G60" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="H60" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="I60" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="J60" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="K60" s="3" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="61" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B61" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C61" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="63" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B63" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="C63" s="5" t="s">
+        <v>26</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>36</v>
+      </c>
+      <c r="H63" s="5"/>
+      <c r="I63" s="5"/>
+      <c r="J63" s="5"/>
+    </row>
+    <row r="64" spans="2:11" x14ac:dyDescent="0.35">
+      <c r="B64" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C64" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G64" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H64" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I64" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J64" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="65" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B65" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="G65" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="H65" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="I65" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J65" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="66" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B66" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C66" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="G66" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="H66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="I66" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="J66" s="3" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="67" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B67" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C67" s="4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="68" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B68" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C68" s="4" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B70" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="C70" s="5"/>
+      <c r="G70" s="5" t="s">
+        <v>61</v>
+      </c>
+      <c r="H70" s="5"/>
+      <c r="I70" s="5"/>
+      <c r="J70" s="5"/>
+    </row>
+    <row r="71" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B71" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C71" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="G71" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H71" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I71" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J71" s="3" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="72" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B72" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="4" t="s">
         <v>56</v>
       </c>
-      <c r="H35" s="8"/>
-      <c r="I35" s="8"/>
-    </row>
-    <row r="36" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="G36" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H36" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I36" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J36" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K36" s="4" t="s">
+      <c r="G72" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="H72" s="3" t="s">
+        <v>63</v>
+      </c>
+      <c r="I72" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="J72" s="3" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="37" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="G37" s="6" t="s">
-        <v>49</v>
-      </c>
-      <c r="H37" s="6" t="s">
-        <v>50</v>
-      </c>
-      <c r="I37" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J37" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K37" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="38" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="G38" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H38" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I38" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K38" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="39" spans="2:11" s="2" customFormat="1" x14ac:dyDescent="0.35"/>
-    <row r="42" spans="2:11" ht="26" x14ac:dyDescent="0.6">
-      <c r="B42" s="3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="45" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B45" s="7" t="s">
-        <v>17</v>
-      </c>
-      <c r="C45" s="7"/>
-      <c r="G45" s="7" t="s">
-        <v>21</v>
-      </c>
-      <c r="H45" s="7"/>
-    </row>
-    <row r="46" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B46" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="G46" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H46" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="47" spans="2:11" x14ac:dyDescent="0.35">
-      <c r="B47" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="G47" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="H47" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="52" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B52" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C52" s="7"/>
-      <c r="D52" s="2"/>
-      <c r="E52" s="2"/>
-      <c r="F52" s="2"/>
-      <c r="G52" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="H52" s="7"/>
-    </row>
-    <row r="53" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B53" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="C53" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="D53" s="2"/>
-      <c r="E53" s="2"/>
-      <c r="F53" s="2"/>
-      <c r="G53" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="H53" s="4" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="54" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B54" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C54" s="4" t="s">
-        <v>37</v>
-      </c>
-      <c r="D54" s="2"/>
-      <c r="E54" s="2"/>
-      <c r="F54" s="2"/>
-      <c r="G54" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="H54" s="4" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="56" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B56" s="7" t="s">
-        <v>31</v>
-      </c>
-      <c r="C56" s="7"/>
-      <c r="P56" s="2"/>
-    </row>
-    <row r="57" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B57" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G57" s="7" t="s">
-        <v>46</v>
-      </c>
-      <c r="H57" s="7"/>
-      <c r="I57" s="7"/>
-      <c r="J57" s="7"/>
-    </row>
-    <row r="58" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B58" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G58" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H58" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I58" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J58" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K58" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="59" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B59" s="4" t="s">
+    <row r="73" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B73" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C59" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G59" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H59" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I59" s="4" t="s">
-        <v>60</v>
-      </c>
-      <c r="J59" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="K59" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="60" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B60" s="4" t="s">
+      <c r="C73" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="G73" s="3">
+        <v>1</v>
+      </c>
+      <c r="H73" s="3" t="s">
+        <v>64</v>
+      </c>
+      <c r="I73" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J73" s="3" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="74" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B74" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C60" s="5" t="s">
+      <c r="C74" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="G60" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="H60" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="I60" s="4" t="s">
-        <v>42</v>
-      </c>
-      <c r="J60" s="4" t="s">
-        <v>43</v>
-      </c>
-      <c r="K60" s="4" t="s">
-        <v>62</v>
-      </c>
-    </row>
-    <row r="61" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B61" s="4" t="s">
+    </row>
+    <row r="75" spans="2:10" x14ac:dyDescent="0.35">
+      <c r="B75" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="C61" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="63" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B63" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="C63" s="7" t="s">
-        <v>26</v>
-      </c>
-      <c r="G63" s="7" t="s">
-        <v>36</v>
-      </c>
-      <c r="H63" s="7"/>
-      <c r="I63" s="7"/>
-      <c r="J63" s="7"/>
-    </row>
-    <row r="64" spans="2:16" x14ac:dyDescent="0.35">
-      <c r="B64" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C64" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G64" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H64" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I64" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="65" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B65" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="G65" s="4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H65" s="4" t="s">
-        <v>45</v>
-      </c>
-      <c r="I65" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J65" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="66" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B66" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C66" s="5" t="s">
-        <v>40</v>
-      </c>
-      <c r="G66" s="4" t="s">
-        <v>0</v>
-      </c>
-      <c r="H66" s="4" t="s">
-        <v>4</v>
-      </c>
-      <c r="I66" s="4" t="s">
-        <v>47</v>
-      </c>
-      <c r="J66" s="4" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="67" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B67" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C67" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="68" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B68" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C68" s="5" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="70" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B70" s="7" t="s">
-        <v>59</v>
-      </c>
-      <c r="C70" s="7"/>
-      <c r="G70" s="7" t="s">
-        <v>63</v>
-      </c>
-      <c r="H70" s="7"/>
-      <c r="I70" s="7"/>
-      <c r="J70" s="7"/>
-    </row>
-    <row r="71" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B71" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C71" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="G71" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H71" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I71" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J71" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="72" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B72" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="C72" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="G72" s="4" t="s">
-        <v>64</v>
-      </c>
-      <c r="H72" s="4" t="s">
-        <v>65</v>
-      </c>
-      <c r="I72" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="J72" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="73" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B73" s="4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C73" s="5" t="s">
-        <v>57</v>
-      </c>
-      <c r="G73" s="4">
-        <v>1</v>
-      </c>
-      <c r="H73" s="4" t="s">
-        <v>66</v>
-      </c>
-      <c r="I73" s="4" t="s">
-        <v>67</v>
-      </c>
-      <c r="J73" s="4" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="74" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B74" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="C74" s="5" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="75" spans="2:10" x14ac:dyDescent="0.35">
-      <c r="B75" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="C75" s="5" t="s">
+      <c r="C75" s="4" t="s">
         <v>25</v>
       </c>
     </row>

</xml_diff>